<commit_message>
ccbottlersus fix add cma isnt_dp
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.7.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Dorit:
+          <t xml:space="preserve">Dorit:
 SSD
  United Deliver</t>
         </r>
@@ -55,7 +55,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Dorit:
+          <t xml:space="preserve">Dorit:
 United Deliver Tea</t>
         </r>
       </text>
@@ -70,7 +70,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Dorit:
+          <t xml:space="preserve">Dorit:
 TEA Category</t>
         </r>
       </text>
@@ -80,355 +80,339 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="110">
-  <si>
-    <t>KPI name</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>scene type</t>
-  </si>
-  <si>
-    <t>template group</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Sparkling</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>CDE Outside Impulse Zone, Cold Vault</t>
-  </si>
-  <si>
-    <t>DASANI/Smartwater</t>
-  </si>
-  <si>
-    <t>DASANI/Smartwater Sparkling</t>
-  </si>
-  <si>
-    <t>Powerade 32oz</t>
-  </si>
-  <si>
-    <t>Powerade 20oz</t>
-  </si>
-  <si>
-    <t>Monster/NOS/Full Throttle</t>
-  </si>
-  <si>
-    <t>Monster Mutant</t>
-  </si>
-  <si>
-    <t>Monster Hydro</t>
-  </si>
-  <si>
-    <t>Minute Maid Juice</t>
-  </si>
-  <si>
-    <t>Minute Maid Refreshment</t>
-  </si>
-  <si>
-    <t>Tum-E-Yummies</t>
-  </si>
-  <si>
-    <t>Tea</t>
-  </si>
-  <si>
-    <t>Huberts Lemonade</t>
-  </si>
-  <si>
-    <t>Vitaminwater</t>
-  </si>
-  <si>
-    <t>Vitaminwater Active</t>
-  </si>
-  <si>
-    <t>Monster JAVA/Cafe</t>
-  </si>
-  <si>
-    <t>Gold Peak Coffee/Latte</t>
-  </si>
-  <si>
-    <t>Dunkin/McCafe</t>
-  </si>
-  <si>
-    <t>Core Power/Monster Muscle?</t>
-  </si>
-  <si>
-    <t>YUP</t>
-  </si>
-  <si>
-    <t>ZICO</t>
-  </si>
-  <si>
-    <t>KPI Name</t>
-  </si>
-  <si>
-    <t>product_ean_code</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Visible</t>
-  </si>
-  <si>
-    <t>7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
-  </si>
-  <si>
-    <t>numerator param 1</t>
-  </si>
-  <si>
-    <t>numerator value 1</t>
-  </si>
-  <si>
-    <t>numerator param 2</t>
-  </si>
-  <si>
-    <t>numerator value 2</t>
-  </si>
-  <si>
-    <t>denominator param 1</t>
-  </si>
-  <si>
-    <t>denominator value 1</t>
-  </si>
-  <si>
-    <t>denominator param 2</t>
-  </si>
-  <si>
-    <t>denominator value 2</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>United Deliver</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>brand_name</t>
-  </si>
-  <si>
-    <t>DASANI WATER,SMARTWATER</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>DASANI SPARKLING,SMARTWATER SPARKLING</t>
-  </si>
-  <si>
-    <t>POWERADE</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>Isotonic</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>MONSTER ENERGY,NOS ENERGY,FULL THROTTLE</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>Monster Energy Mutant Green,Monster Energy Mutant Red,Monster Mutant Super Soda White Lightning Zero Sugar 20 fl oz</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>MONSTER HYDRO Tropical Thunder 12/25.4oz,MONSTER HYDRO Purple Passion 12/25.4oz,MONSTER HYDRO Blue Ice 12/25.4oz,MONSTER HYDRO Zero Sugar 12/25.4oz,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Monster Hydro Manic Melon 16.9oz,Monster Hydro Mean Green 16.9oz,Monster Hydro Tropical Thunder 16.9oz</t>
-    </r>
-  </si>
-  <si>
-    <t>MINUTE MAID</t>
-  </si>
-  <si>
-    <t>Juice</t>
-  </si>
-  <si>
-    <t>Minute Maid Refreshment Lemonade 12 fl oz  X 6,Minute Maid Refreshment Lemonade 12 fl oz,Minute M Refreshments Watermelon Punch 20 OZ PET,Minute M Refreshments Watermelon Punch 2-Liter,Minute M Refreshments Watermelon Punch Fridgepack</t>
-  </si>
-  <si>
-    <t>Tum-E Yummies</t>
-  </si>
-  <si>
-    <t>Hubert's</t>
-  </si>
-  <si>
-    <t>GLACEAU VITAMIN WATER</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>Enhanced</t>
-  </si>
-  <si>
-    <t>Vitamin Water Active Pump It 15.2 FL OZ PET,Vitamin Water Active Werk It 15.2 FL OZ PET,Vitamin Water Active Move It 15.2 FL OZ PET</t>
-  </si>
-  <si>
-    <t>MONSTER COFFEE+ENERGY</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>GOLD PEAK COFFEE</t>
-  </si>
-  <si>
-    <t>DUNKIN DONUTS,MC CAFE</t>
-  </si>
-  <si>
-    <t>CORE POWER</t>
-  </si>
-  <si>
-    <t>Monster Energy Muscle Peanut Butter Cup Energy Shakes 15oz 4pack,Monster Energy Muscle Vanilla Energy Shakes,Monster Energy Muscle Monster Vanilla 16oz,Monster Energy Muscle Monster Chocolate 16oz,MONSTER Muscle Monster Chocolate 12/15oz,MONSTER Muscle Monster Vanilla 12/15oz</t>
-  </si>
-  <si>
-    <t>SHELF STABLE PROTEIN</t>
-  </si>
-  <si>
-    <t>SHELF STABLE DAIRY</t>
-  </si>
-  <si>
-    <t>ZICO COCONUT WATER</t>
-  </si>
-  <si>
-    <t>Coconut water</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>program</t>
-  </si>
-  <si>
-    <t>sales center</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>UNITED</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Baton Rouge</t>
-  </si>
-  <si>
-    <t>CR&amp;LT</t>
-  </si>
-  <si>
-    <t>Baton Rouge Black</t>
-  </si>
-  <si>
-    <t>Confirmed by Steve:</t>
-  </si>
-  <si>
-    <t>SOVI KPI</t>
-  </si>
-  <si>
-    <t>Numerator</t>
-  </si>
-  <si>
-    <t>Denominator </t>
-  </si>
-  <si>
-    <t>Coke United SSD</t>
-  </si>
-  <si>
-    <t>SSD Category</t>
-  </si>
-  <si>
-    <t>Water </t>
-  </si>
-  <si>
-    <t> Water</t>
-  </si>
-  <si>
-    <t> Isotonic</t>
-  </si>
-  <si>
-    <t> Energy</t>
-  </si>
-  <si>
-    <t> Energy – SSD category</t>
-  </si>
-  <si>
-    <t> Juice </t>
-  </si>
-  <si>
-    <t> Juice – 20 oz 3% MMR is SSD category.</t>
-  </si>
-  <si>
-    <t> RTD Tea</t>
-  </si>
-  <si>
-    <t> Juice</t>
-  </si>
-  <si>
-    <t> Enhanced Water</t>
-  </si>
-  <si>
-    <t>Monster JAVA/Café</t>
-  </si>
-  <si>
-    <t> RTD Coffee ?  Correct.</t>
-  </si>
-  <si>
-    <t> RTD Coffee</t>
-  </si>
-  <si>
-    <t> Energy?  Protein</t>
-  </si>
-  <si>
-    <t> ?  shelf stable dairy</t>
-  </si>
-  <si>
-    <t> Coconut Water</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="111">
+  <si>
+    <t xml:space="preserve">KPI name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparkling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDE Outside Impulse Zone, Cold Vault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DASANI/Smartwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DASANI/Smartwater Sparkling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powerade 32oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powerade 20oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster/NOS/Full Throttle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Mutant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Hydro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minute Maid Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minute Maid Refreshment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tum-E-Yummies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huberts Lemonade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitaminwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitaminwater Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster JAVA/Cafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold Peak Coffee/Latte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunkin/McCafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Power/Monster Muscle?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_ean_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Deliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DASANI WATER,SMARTWATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DASANI SPARKLING,SMARTWATER SPARKLING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER ENERGY,NOS ENERGY,FULL THROTTLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Energy Mutant Green,Monster Energy Mutant Red,Monster Mutant Super Soda White Lightning Zero Sugar 20 fl oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER HYDRO Tropical Thunder 12/25.4oz,MONSTER HYDRO Purple Passion 12/25.4oz,MONSTER HYDRO Blue Ice 12/25.4oz,MONSTER HYDRO Zero Sugar 12/25.4oz,Monster Hydro Manic Melon 16.9oz,Monster Hydro Mean Green 16.9oz,Monster Hydro Tropical Thunder 16.9oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINUTE MAID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minute Maid Refreshment Lemonade 12 fl oz  X 6,Minute Maid Refreshment Lemonade 12 fl oz,Minute M Refreshments Watermelon Punch 20 OZ PET,Minute M Refreshments Watermelon Punch 2-Liter,Minute M Refreshments Watermelon Punch Fridgepack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tum-E Yummies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hubert's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLACEAU VITAMIN WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin Water Active Pump It 15.2 FL OZ PET,Vitamin Water Active Werk It 15.2 FL OZ PET,Vitamin Water Active Move It 15.2 FL OZ PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER COFFEE+ENERGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOLD PEAK COFFEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUNKIN DONUTS,MC CAFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORE POWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Energy Muscle Peanut Butter Cup Energy Shakes 15oz 4pack,Monster Energy Muscle Vanilla Energy Shakes,Monster Energy Muscle Monster Vanilla 16oz,Monster Energy Muscle Monster Chocolate 16oz,MONSTER Muscle Monster Chocolate 12/15oz,MONSTER Muscle Monster Vanilla 12/15oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF STABLE PROTEIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF STABLE DAIRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZICO COCONUT WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coconut water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sales center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baton Rouge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baton Rouge Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmed by Steve:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOVI KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coke United SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isotonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Energy – SSD category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juice </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juice – 20 oz 3% MMR is SSD category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RTD Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enhanced Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster JAVA/Café</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RTD Coffee ?  Correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RTD Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Energy?  Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ?  shelf stable dairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coconut Water</t>
   </si>
 </sst>
 </file>
@@ -436,7 +420,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
@@ -726,7 +710,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -906,9 +890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1127520</xdr:colOff>
+      <xdr:colOff>1127160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -918,7 +902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="7961400" cy="6348960"/>
+          <a:ext cx="8008920" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -951,9 +935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1127520</xdr:colOff>
+      <xdr:colOff>1127160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -963,7 +947,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="7961400" cy="6348960"/>
+          <a:ext cx="8008920" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,9 +980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1127520</xdr:colOff>
+      <xdr:colOff>1127160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1008,7 +992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="7961400" cy="6348960"/>
+          <a:ext cx="8008920" cy="6348600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,23 +1026,23 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5263157894737"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5182186234818"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1074,241 +1058,244 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1323,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.5627530364373"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1345,21 +1332,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="70.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>1</v>
@@ -1383,97 +1370,97 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.5546558704453"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="39.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G2" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -1482,21 +1469,21 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
@@ -1505,25 +1492,25 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
@@ -1532,25 +1519,25 @@
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>52</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -1559,21 +1546,21 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
@@ -1582,21 +1569,21 @@
     </row>
     <row r="8" customFormat="false" ht="77.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="10"/>
@@ -1605,21 +1592,21 @@
     </row>
     <row r="9" customFormat="false" ht="151.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -1628,21 +1615,21 @@
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -1651,21 +1638,21 @@
     </row>
     <row r="11" customFormat="false" ht="136.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -1674,21 +1661,21 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -1697,19 +1684,19 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -1718,207 +1705,207 @@
     </row>
     <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="77.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="246.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
       <c r="F21" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
       <c r="F22" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1945,11 +1932,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1958,36 +1945,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F2" s="33" t="n">
         <v>1</v>
@@ -1995,19 +1982,19 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F3" s="33" t="n">
         <v>0.9</v>
@@ -2015,19 +2002,19 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F4" s="33" t="n">
         <v>0.9</v>
@@ -2035,19 +2022,19 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F5" s="33" t="n">
         <v>0.9</v>
@@ -2055,19 +2042,19 @@
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F6" s="33" t="n">
         <v>0.9</v>
@@ -2075,19 +2062,19 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F7" s="33" t="n">
         <v>0.9</v>
@@ -2095,19 +2082,19 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F8" s="33" t="n">
         <v>0.9</v>
@@ -2115,19 +2102,19 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F9" s="33" t="n">
         <v>0.9</v>
@@ -2135,19 +2122,19 @@
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F10" s="33" t="n">
         <v>0.9</v>
@@ -2155,19 +2142,19 @@
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F11" s="33" t="n">
         <v>0.9</v>
@@ -2175,19 +2162,19 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F12" s="33" t="n">
         <v>0.9</v>
@@ -2195,19 +2182,19 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F13" s="33" t="n">
         <v>0.9</v>
@@ -2215,19 +2202,19 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F14" s="33" t="n">
         <v>0.9</v>
@@ -2235,19 +2222,19 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="33" t="n">
         <v>0.9</v>
@@ -2255,19 +2242,19 @@
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="33" t="n">
         <v>0.9</v>
@@ -2275,19 +2262,19 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F17" s="33" t="n">
         <v>0.9</v>
@@ -2295,19 +2282,19 @@
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F18" s="33" t="n">
         <v>0.9</v>
@@ -2315,19 +2302,19 @@
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="33" t="n">
         <v>0.9</v>
@@ -2335,19 +2322,19 @@
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="33" t="n">
         <v>0.9</v>
@@ -2355,19 +2342,19 @@
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" s="33" t="n">
         <v>0.9</v>
@@ -2375,19 +2362,19 @@
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F22" s="33" t="n">
         <v>0.9</v>
@@ -2395,19 +2382,19 @@
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F23" s="33" t="n">
         <v>0.8</v>
@@ -2415,19 +2402,19 @@
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F24" s="33" t="n">
         <v>0.6</v>
@@ -2435,19 +2422,19 @@
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F25" s="33" t="n">
         <v>0.6</v>
@@ -2455,19 +2442,19 @@
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F26" s="33" t="n">
         <v>0.6</v>
@@ -2475,19 +2462,19 @@
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F27" s="33" t="n">
         <v>0.6</v>
@@ -2495,19 +2482,19 @@
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F28" s="33" t="n">
         <v>0.6</v>
@@ -2515,19 +2502,19 @@
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F29" s="33" t="n">
         <v>0.6</v>
@@ -2535,19 +2522,19 @@
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F30" s="33" t="n">
         <v>0.6</v>
@@ -2555,19 +2542,19 @@
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F31" s="33" t="n">
         <v>0.6</v>
@@ -2575,19 +2562,19 @@
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F32" s="33" t="n">
         <v>0.6</v>
@@ -2595,19 +2582,19 @@
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F33" s="33" t="n">
         <v>0.6</v>
@@ -2615,19 +2602,19 @@
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F34" s="33" t="n">
         <v>0.6</v>
@@ -2635,19 +2622,19 @@
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F35" s="33" t="n">
         <v>0.6</v>
@@ -2655,19 +2642,19 @@
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F36" s="33" t="n">
         <v>0.6</v>
@@ -2675,19 +2662,19 @@
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F37" s="33" t="n">
         <v>0.6</v>
@@ -2695,19 +2682,19 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F38" s="33" t="n">
         <v>0.6</v>
@@ -2715,19 +2702,19 @@
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F39" s="33" t="n">
         <v>0.6</v>
@@ -2735,19 +2722,19 @@
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F40" s="33" t="n">
         <v>0.6</v>
@@ -2755,19 +2742,19 @@
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F41" s="33" t="n">
         <v>0.6</v>
@@ -2775,19 +2762,19 @@
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F42" s="33" t="n">
         <v>0.6</v>
@@ -2795,19 +2782,19 @@
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F43" s="33" t="n">
         <v>0.6</v>
@@ -2837,255 +2824,255 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>